<commit_message>
updates on example import files
</commit_message>
<xml_diff>
--- a/public/User import example_en.xlsx
+++ b/public/User import example_en.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nghia.dnn\Desktop\Appartment-Management-System-Server\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Appartment-Management-System-Server\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E605955-00FF-440B-BBD2-38D4F7187845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6377C2C2-C7D9-47D0-B25E-4A9A2874B57D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1965" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
   <si>
     <t>Email</t>
   </si>
@@ -112,6 +112,24 @@
   </si>
   <si>
     <t>test123@gmail.com</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>123456789005</t>
+  </si>
+  <si>
+    <t>123456005</t>
+  </si>
+  <si>
+    <t>test456@gmail.com</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
@@ -453,7 +471,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -612,6 +630,56 @@
         <v>0</v>
       </c>
     </row>
+    <row r="4" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="3">
+        <v>36526</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="2">
+        <v>123456</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O4" s="2">
+        <v>0</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1" xr:uid="{83819D46-F3DF-468D-88C5-FF03F1737EB3}"/>
@@ -622,6 +690,10 @@
     <hyperlink ref="K3" r:id="rId6" xr:uid="{823CB157-61A5-46AD-9336-BF7D144DF53F}"/>
     <hyperlink ref="L3" r:id="rId7" xr:uid="{7F033203-0AFB-4A58-862E-64B97630948E}"/>
     <hyperlink ref="M3" r:id="rId8" xr:uid="{08F40C62-6835-4DFD-B5DF-FBE4A11BB2C2}"/>
+    <hyperlink ref="H4" r:id="rId9" xr:uid="{211009E9-1290-45D0-BC73-148FC6622594}"/>
+    <hyperlink ref="K4" r:id="rId10" xr:uid="{470EE76C-07F7-4777-9AA8-E3569EAFEB21}"/>
+    <hyperlink ref="L4" r:id="rId11" xr:uid="{44851BE5-6413-4FCD-A5D2-57D9BD359659}"/>
+    <hyperlink ref="M4" r:id="rId12" xr:uid="{A85076EC-DF86-4FC3-A08F-C033C1351D6C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
finished building models and migrations code for the database (#1)
</commit_message>
<xml_diff>
--- a/public/User import example_en.xlsx
+++ b/public/User import example_en.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nghia.dnn\Desktop\Appartment-Management-System-Server\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Appartment-Management-System-Server\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E605955-00FF-440B-BBD2-38D4F7187845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6377C2C2-C7D9-47D0-B25E-4A9A2874B57D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1965" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
   <si>
     <t>Email</t>
   </si>
@@ -112,6 +112,24 @@
   </si>
   <si>
     <t>test123@gmail.com</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>123456789005</t>
+  </si>
+  <si>
+    <t>123456005</t>
+  </si>
+  <si>
+    <t>test456@gmail.com</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
@@ -453,7 +471,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -612,6 +630,56 @@
         <v>0</v>
       </c>
     </row>
+    <row r="4" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="3">
+        <v>36526</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="2">
+        <v>123456</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O4" s="2">
+        <v>0</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1" xr:uid="{83819D46-F3DF-468D-88C5-FF03F1737EB3}"/>
@@ -622,6 +690,10 @@
     <hyperlink ref="K3" r:id="rId6" xr:uid="{823CB157-61A5-46AD-9336-BF7D144DF53F}"/>
     <hyperlink ref="L3" r:id="rId7" xr:uid="{7F033203-0AFB-4A58-862E-64B97630948E}"/>
     <hyperlink ref="M3" r:id="rId8" xr:uid="{08F40C62-6835-4DFD-B5DF-FBE4A11BB2C2}"/>
+    <hyperlink ref="H4" r:id="rId9" xr:uid="{211009E9-1290-45D0-BC73-148FC6622594}"/>
+    <hyperlink ref="K4" r:id="rId10" xr:uid="{470EE76C-07F7-4777-9AA8-E3569EAFEB21}"/>
+    <hyperlink ref="L4" r:id="rId11" xr:uid="{44851BE5-6413-4FCD-A5D2-57D9BD359659}"/>
+    <hyperlink ref="M4" r:id="rId12" xr:uid="{A85076EC-DF86-4FC3-A08F-C033C1351D6C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Merge from dev for testing
</commit_message>
<xml_diff>
--- a/public/User import example_en.xlsx
+++ b/public/User import example_en.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nghia.dnn\Desktop\Appartment-Management-System-Server\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Appartment-Management-System-Server\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E605955-00FF-440B-BBD2-38D4F7187845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6377C2C2-C7D9-47D0-B25E-4A9A2874B57D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1965" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
   <si>
     <t>Email</t>
   </si>
@@ -112,6 +112,24 @@
   </si>
   <si>
     <t>test123@gmail.com</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>123456789005</t>
+  </si>
+  <si>
+    <t>123456005</t>
+  </si>
+  <si>
+    <t>test456@gmail.com</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
@@ -453,7 +471,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -612,6 +630,56 @@
         <v>0</v>
       </c>
     </row>
+    <row r="4" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="3">
+        <v>36526</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="2">
+        <v>123456</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O4" s="2">
+        <v>0</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1" xr:uid="{83819D46-F3DF-468D-88C5-FF03F1737EB3}"/>
@@ -622,6 +690,10 @@
     <hyperlink ref="K3" r:id="rId6" xr:uid="{823CB157-61A5-46AD-9336-BF7D144DF53F}"/>
     <hyperlink ref="L3" r:id="rId7" xr:uid="{7F033203-0AFB-4A58-862E-64B97630948E}"/>
     <hyperlink ref="M3" r:id="rId8" xr:uid="{08F40C62-6835-4DFD-B5DF-FBE4A11BB2C2}"/>
+    <hyperlink ref="H4" r:id="rId9" xr:uid="{211009E9-1290-45D0-BC73-148FC6622594}"/>
+    <hyperlink ref="K4" r:id="rId10" xr:uid="{470EE76C-07F7-4777-9AA8-E3569EAFEB21}"/>
+    <hyperlink ref="L4" r:id="rId11" xr:uid="{44851BE5-6413-4FCD-A5D2-57D9BD359659}"/>
+    <hyperlink ref="M4" r:id="rId12" xr:uid="{A85076EC-DF86-4FC3-A08F-C033C1351D6C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>